<commit_message>
RFM, EDA, merge file, Kmeans etc... => 50%
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_5\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF34696-FBB6-48CE-A8FF-43C444411294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3108F155-66C3-4D73-85C8-6E37B903B20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -60,17 +60,68 @@
     <t>Évaluer les performances d’un modèle d'apprentissage non supervisé</t>
   </si>
   <si>
-    <t>Feature selection / engeneering</t>
-  </si>
-  <si>
-    <t>Analyse exploratoire</t>
+    <t>Les variables pertinentes ont été transformées pour permettre leur exploitation (variables catégorielles en particulier).</t>
+  </si>
+  <si>
+    <t>Une ou plusieurs variables pertinentes permettant d'améliorer la solution proposée ont été créées.</t>
+  </si>
+  <si>
+    <t>Le nombre de segments et la répartition est adapté à la problématique métier.</t>
+  </si>
+  <si>
+    <t>La stratégie d'ajout de nouveaux clients a été explicitée.</t>
+  </si>
+  <si>
+    <t>La nature des variables d'entrée a été prise en compte dans le choix de l'algorithme et de la distance.</t>
+  </si>
+  <si>
+    <t>La forme des clusters est évaluée.</t>
+  </si>
+  <si>
+    <t>La stabilité des clusters est évaluée.</t>
+  </si>
+  <si>
+    <t>La compatibilité avec des connaissances extérieures est évaluée ("test set" et/ou a priori).</t>
+  </si>
+  <si>
+    <t>Les étapes d'évaluation sont automatisées pour tester facilement plusieurs combinaisons de paramètres.</t>
+  </si>
+  <si>
+    <t>Les valeurs de paramètres testés sont pertinemment choisies.</t>
+  </si>
+  <si>
+    <t>Respecter la convention PEP8 (facultatif)</t>
+  </si>
+  <si>
+    <t>La convention pep8 est respectée</t>
+  </si>
+  <si>
+    <t>Le code est commentée (commentaires réguliers, docstrings dans les fonctions)</t>
+  </si>
+  <si>
+    <t>Pep convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Méthode du coude</t>
+  </si>
+  <si>
+    <t>Silhouette-score</t>
+  </si>
+  <si>
+    <t>RFM test avec les segment définie avec les quartiles</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +168,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Montserrat"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +224,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -206,7 +258,37 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -216,35 +298,39 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -254,30 +340,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -286,16 +348,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -305,7 +374,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -314,14 +383,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -331,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,20 +406,30 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -360,35 +437,43 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -684,128 +769,221 @@
     <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15" thickBot="1"/>
-    <row r="3" spans="2:6" ht="21.5" customHeight="1" thickBot="1">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1"/>
+    <row r="3" spans="2:8" ht="21.5" customHeight="1" thickBot="1">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="39" customHeight="1" thickBot="1">
-      <c r="B4" s="19" t="s">
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="39" customHeight="1" thickBot="1">
+      <c r="B4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="3">
+        <f>AVERAGE(C5:C7,C9:C11,C13:C15,C17:C18,)</f>
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="H4" s="3">
+        <f>AVERAGE(C20:C21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="56.5" customHeight="1">
+      <c r="B5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:8" ht="56.5" customHeight="1">
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="2:8" ht="56.5" customHeight="1" thickBot="1">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="C7" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="2:8" ht="52" customHeight="1">
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" ht="52" customHeight="1">
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13">
         <v>0</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="52" customHeight="1" thickBot="1">
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="2:8" ht="42.5" customHeight="1">
+      <c r="B13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="42.5" customHeight="1">
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="2:8" ht="55" customHeight="1" thickBot="1">
+      <c r="B15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B16" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="2:4" ht="56.5" customHeight="1">
+      <c r="B17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="2:4" ht="56.5" customHeight="1" thickBot="1">
+      <c r="B18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="2:4" ht="42.5" customHeight="1">
+      <c r="B20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="12">
         <v>0</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="F6" s="5">
-        <f>AVERAGE(C5:C7,C9:C9,C11:C11,C13:C13)</f>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="2:4" ht="42.5" customHeight="1" thickBot="1">
+      <c r="B21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0</v>
-      </c>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="2:6" ht="65.5" customHeight="1" thickBot="1">
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B12" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="2:6" ht="42.5" customHeight="1">
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="2:6" ht="27.5" customHeight="1">
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="2:6" ht="27.5" customHeight="1" thickBot="1">
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="2:6" ht="27.5" customHeight="1"/>
-    <row r="17" ht="27.5" customHeight="1"/>
-    <row r="18" ht="27.5" customHeight="1"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="23" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="24" spans="2:4" ht="27.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B10:C10"/>
+  <mergeCells count="5">
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
-  <conditionalFormatting sqref="C11 C13 C5:C7 C9">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="C5:C7 C9:C11 C13:C15 C17:C18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color theme="5"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C21">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>

</xml_diff>

<commit_message>
Clustering in progress, Evaluation and stability
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_5\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3108F155-66C3-4D73-85C8-6E37B903B20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60A95A3-F5C2-4CD5-AA7F-9F91827ACC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -108,13 +108,16 @@
     <t>Méthode du coude</t>
   </si>
   <si>
-    <t>Silhouette-score</t>
-  </si>
-  <si>
     <t>RFM test avec les segment définie avec les quartiles</t>
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Silhouette-score et sample silhouette</t>
+  </si>
+  <si>
+    <t>Ari_Score sur 12 mois</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
   <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -798,7 +801,7 @@
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C7,C9:C11,C13:C15,C17:C18,)</f>
-        <v>0.47500000000000003</v>
+        <v>0.63333333333333341</v>
       </c>
       <c r="H4" s="3">
         <f>AVERAGE(C20:C21)</f>
@@ -828,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="14">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -844,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="12">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -856,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -867,7 +870,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="14">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D11" s="10"/>
     </row>
@@ -883,10 +886,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="12">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="42.5" customHeight="1">
@@ -894,19 +897,21 @@
         <v>14</v>
       </c>
       <c r="C14" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="55" customHeight="1" thickBot="1">
       <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="14">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
@@ -930,7 +935,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="14">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Simple clustering done, Stability and new client in progress => 75-80%
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_5\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60A95A3-F5C2-4CD5-AA7F-9F91827ACC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0209A39-7D27-4422-A1ED-6486119CB2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,19 +105,19 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Méthode du coude</t>
-  </si>
-  <si>
     <t>RFM test avec les segment définie avec les quartiles</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Silhouette-score et sample silhouette</t>
   </si>
   <si>
     <t>Ari_Score sur 12 mois</t>
+  </si>
+  <si>
+    <t>Méthode du coude silhouette sample</t>
+  </si>
+  <si>
+    <t>Mettre  plus de méthode sur les étape de clustering et le faire avec le DBScan</t>
   </si>
 </sst>
 </file>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -801,11 +801,11 @@
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C7,C9:C11,C13:C15,C17:C18,)</f>
-        <v>0.63333333333333341</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="H4" s="3">
         <f>AVERAGE(C20:C21)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="56.5" customHeight="1">
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -831,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -847,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="12">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -856,11 +856,9 @@
         <v>11</v>
       </c>
       <c r="C10" s="13">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="4"/>
       <c r="F10" t="s">
         <v>22</v>
       </c>
@@ -870,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D11" s="10"/>
     </row>
@@ -886,10 +884,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="12">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="42.5" customHeight="1">
@@ -897,10 +895,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="55" customHeight="1" thickBot="1">
@@ -911,7 +909,7 @@
         <v>0.8</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
@@ -926,9 +924,11 @@
         <v>16</v>
       </c>
       <c r="C17" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="D17" s="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="56.5" customHeight="1" thickBot="1">
       <c r="B18" s="11" t="s">
@@ -938,7 +938,7 @@
         <v>0.7</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
@@ -953,7 +953,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D20" s="6"/>
     </row>
@@ -962,7 +962,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="16">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D21" s="11"/>
     </row>

</xml_diff>

<commit_message>
add new client done and clustering with PCA done, slide presentation in progress.
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_5\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0209A39-7D27-4422-A1ED-6486119CB2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BD8C24-9F56-4ECC-A117-8A9F593114E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -105,19 +105,37 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>RFM test avec les segment définie avec les quartiles</t>
-  </si>
-  <si>
     <t>Silhouette-score et sample silhouette</t>
   </si>
   <si>
-    <t>Ari_Score sur 12 mois</t>
-  </si>
-  <si>
-    <t>Méthode du coude silhouette sample</t>
-  </si>
-  <si>
-    <t>Mettre  plus de méthode sur les étape de clustering et le faire avec le DBScan</t>
+    <t>A faire avec l'ajout de nouveaux clients</t>
+  </si>
+  <si>
+    <t>Review_score_evolution, RFM etc..</t>
+  </si>
+  <si>
+    <t>Kmeans car le reste pas vraiment adaptée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ari_Score sur 12 mois et stabilité avec davies_bouldin </t>
+  </si>
+  <si>
+    <t>Méthode du coude silhouette sample, davies_bouldin + GridSearchCV</t>
+  </si>
+  <si>
+    <t>Test fait mais pas implémenté car pas nécessaire</t>
+  </si>
+  <si>
+    <t>Docstring dans les fonctions et commentaire régulier</t>
+  </si>
+  <si>
+    <t>Reste encore l'indentation</t>
+  </si>
+  <si>
+    <t>Méthode de test cluster Kmeans et GridSearch perso pour le DBScan</t>
+  </si>
+  <si>
+    <t>2 méthodes</t>
   </si>
 </sst>
 </file>
@@ -762,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -800,12 +818,12 @@
       <c r="C4" s="22"/>
       <c r="D4" s="7"/>
       <c r="F4" s="3">
-        <f>AVERAGE(C5:C7,C9:C11,C13:C15,C17:C18,)</f>
-        <v>0.79166666666666663</v>
+        <f>AVERAGE(C5:C7,C9:C11,C13:C15,C17:C18)</f>
+        <v>1</v>
       </c>
       <c r="H4" s="3">
         <f>AVERAGE(C20:C21)</f>
-        <v>0.3</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="56.5" customHeight="1">
@@ -815,7 +833,9 @@
       <c r="C5" s="12">
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="2:8" ht="56.5" customHeight="1">
       <c r="B6" s="5" t="s">
@@ -824,7 +844,9 @@
       <c r="C6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="2:8" ht="56.5" customHeight="1" thickBot="1">
       <c r="B7" s="11" t="s">
@@ -833,7 +855,9 @@
       <c r="C7" s="14">
         <v>1</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
       <c r="B8" s="19" t="s">
@@ -856,9 +880,11 @@
         <v>11</v>
       </c>
       <c r="C10" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
@@ -887,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="42.5" customHeight="1">
@@ -898,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="55" customHeight="1" thickBot="1">
@@ -906,10 +932,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
@@ -924,10 +950,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="56.5" customHeight="1" thickBot="1">
@@ -935,10 +961,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="14">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
@@ -953,18 +979,22 @@
         <v>19</v>
       </c>
       <c r="C20" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="2:4" ht="42.5" customHeight="1" thickBot="1">
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="D21" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="2:4" ht="27.5" customHeight="1"/>
     <row r="23" spans="2:4" ht="27.5" customHeight="1"/>

</xml_diff>